<commit_message>
daca and bulk contracts implmeneted
</commit_message>
<xml_diff>
--- a/deterministic_2cust_2mills.xlsx
+++ b/deterministic_2cust_2mills.xlsx
@@ -1,37 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Thesis\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B18750D-8F1D-4A63-AA78-A8C916FA23C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C1C04E-B162-419D-879B-3C3B04B1823F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{B617CF86-C715-45AA-82CA-B7528EBD08D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="9" activeTab="11" xr2:uid="{B617CF86-C715-45AA-82CA-B7528EBD08D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Contracts" sheetId="14" r:id="rId1"/>
-    <sheet name="DACA_limits" sheetId="16" r:id="rId2"/>
-    <sheet name="DACA_prices" sheetId="15" r:id="rId3"/>
-    <sheet name="PM" sheetId="10" r:id="rId4"/>
-    <sheet name="CustomerDemand" sheetId="1" r:id="rId5"/>
-    <sheet name="FixedCosts" sheetId="2" r:id="rId6"/>
-    <sheet name="RawMaterialConversion" sheetId="12" r:id="rId7"/>
-    <sheet name="RawMaterialPrices" sheetId="13" r:id="rId8"/>
-    <sheet name="RawMaterialCosts" sheetId="7" r:id="rId9"/>
-    <sheet name="ShutdownCosts" sheetId="3" r:id="rId10"/>
-    <sheet name="Capacity" sheetId="4" r:id="rId11"/>
-    <sheet name="LogisticCosts" sheetId="5" r:id="rId12"/>
-    <sheet name="StorageCapacities" sheetId="11" r:id="rId13"/>
-    <sheet name="StorageCosts" sheetId="6" r:id="rId14"/>
-    <sheet name="Prices" sheetId="8" r:id="rId15"/>
-    <sheet name="EnergyCosts" sheetId="9" r:id="rId16"/>
+    <sheet name="BULK_prices" sheetId="18" r:id="rId2"/>
+    <sheet name="BULK_limits" sheetId="17" r:id="rId3"/>
+    <sheet name="DACA_limits" sheetId="16" r:id="rId4"/>
+    <sheet name="DACA_prices" sheetId="15" r:id="rId5"/>
+    <sheet name="PM" sheetId="10" r:id="rId6"/>
+    <sheet name="CustomerDemand" sheetId="1" r:id="rId7"/>
+    <sheet name="FixedCosts" sheetId="2" r:id="rId8"/>
+    <sheet name="RawMaterialConversion" sheetId="12" r:id="rId9"/>
+    <sheet name="RawMaterialPrices" sheetId="13" r:id="rId10"/>
+    <sheet name="ShutdownCosts" sheetId="3" r:id="rId11"/>
+    <sheet name="Capacity" sheetId="4" r:id="rId12"/>
+    <sheet name="LogisticCosts" sheetId="5" r:id="rId13"/>
+    <sheet name="StorageCapacities" sheetId="11" r:id="rId14"/>
+    <sheet name="StorageCosts" sheetId="6" r:id="rId15"/>
+    <sheet name="Prices" sheetId="8" r:id="rId16"/>
+    <sheet name="EnergyCosts" sheetId="9" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">CustomerDemand!$A$1:$D$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">CustomerDemand!$A$1:$D$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="27">
   <si>
     <t>CALMONTH</t>
   </si>
@@ -125,6 +126,15 @@
   </si>
   <si>
     <t>d2</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>BULK</t>
   </si>
 </sst>
 </file>
@@ -483,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13C6E192-1665-4CDB-9DF2-851F1DEF180F}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,12 +519,180 @@
         <v>19</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD32A2A-87A0-4F8D-AE5A-93ADC2EEC530}">
+  <dimension ref="A1:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>202201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>202202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>202203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>202204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>202205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>202206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>202207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>202208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>202209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>202210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>202211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>202212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F0B721C-577B-451B-A2D9-B0C235329D77}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -557,12 +735,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056091E-ED20-4BE9-BFB5-D2E8FBB81DC4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +777,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70140EC5-C154-495E-B51C-01385B805036}">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -673,7 +851,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7405781-B97C-4E23-8490-ED76820794D0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -712,7 +890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39B2EE5-405F-4405-87E0-62869557828C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -754,12 +932,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78DFDA0-7BB8-481E-ABDA-D7E93FE004F8}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,12 +1095,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DA63832-DF2E-42DF-9C94-194CC94CEF5F}">
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,7 +1345,7 @@
         <v>11</v>
       </c>
       <c r="E14">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1184,7 +1362,7 @@
         <v>11</v>
       </c>
       <c r="E15">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,7 +1379,7 @@
         <v>11</v>
       </c>
       <c r="E16">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,7 +1396,7 @@
         <v>11</v>
       </c>
       <c r="E17">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,7 +1413,7 @@
         <v>11</v>
       </c>
       <c r="E18">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,7 +1430,7 @@
         <v>11</v>
       </c>
       <c r="E19">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,7 +1447,7 @@
         <v>11</v>
       </c>
       <c r="E20">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1286,7 +1464,7 @@
         <v>11</v>
       </c>
       <c r="E21">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,7 +1481,7 @@
         <v>11</v>
       </c>
       <c r="E22">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1320,7 +1498,7 @@
         <v>11</v>
       </c>
       <c r="E23">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1337,7 +1515,7 @@
         <v>11</v>
       </c>
       <c r="E24">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,7 +1532,7 @@
         <v>11</v>
       </c>
       <c r="E25">
-        <v>1000000</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1364,11 +1542,1011 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6B24168-5D53-4AA9-B9F9-CF4AA55A7492}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>202201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>202202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>202203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>202204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>202205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>202206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>202207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>202208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>202209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>202210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>202211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>202212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>202201</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>202202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>202203</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>202204</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>202205</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>202206</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>202207</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>202208</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>202209</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>202210</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>202211</v>
+      </c>
+      <c r="B24" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>202212</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>202201</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>202202</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>202203</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>202204</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>202205</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>202206</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>202207</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>202208</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>202209</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>202210</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>202211</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C36" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>202212</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>202201</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>202202</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>202203</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>202204</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>202205</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>202206</v>
+      </c>
+      <c r="B43" t="s">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>202207</v>
+      </c>
+      <c r="B44" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>202208</v>
+      </c>
+      <c r="B45" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>202209</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>202210</v>
+      </c>
+      <c r="B47" t="s">
+        <v>25</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>202211</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>202212</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97DD519D-FCAE-4565-A8E9-54C12B69E431}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>202201</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>202202</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>202203</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>202204</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>202205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>202206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>202207</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>202208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>202209</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>202210</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>202211</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>202212</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>202201</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>202202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>202203</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>202204</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>202205</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>202206</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>202207</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>202208</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>202209</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>202210</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>202211</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>202212</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DB3DDE-A9BE-40EC-AE3F-6355B52266C4}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +2575,7 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>1.4440010051454788</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1408,7 +2586,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>47.53387271334244</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1419,7 +2597,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>44.937648838224987</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1430,7 +2608,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>35.435088603181562</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1441,7 +2619,7 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>7.2827297936178201</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1452,7 +2630,7 @@
         <v>10</v>
       </c>
       <c r="C7">
-        <v>3.1853719901490885</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1463,7 +2641,7 @@
         <v>10</v>
       </c>
       <c r="C8">
-        <v>9.0311330800081304</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1474,7 +2652,7 @@
         <v>10</v>
       </c>
       <c r="C9">
-        <v>13.613991042691332</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1485,7 +2663,7 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>12.764754481010826</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1496,7 +2674,7 @@
         <v>10</v>
       </c>
       <c r="C11">
-        <v>17.054959293347299</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1507,7 +2685,7 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>6.3859810587668155</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1518,7 +2696,7 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>41.797094873665145</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1529,7 +2707,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>35.893503848335889</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1540,7 +2718,7 @@
         <v>10</v>
       </c>
       <c r="C15">
-        <v>7.6447065120742064</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1551,7 +2729,7 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>18.799422456427461</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1562,7 +2740,7 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>4.6016675220618533</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1573,7 +2751,7 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>1.8674222000847507</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1584,7 +2762,7 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>40.518774319499826</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1595,7 +2773,7 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <v>25.96471267852079</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1606,7 +2784,7 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>23.32947948295816</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1617,7 +2795,7 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>40.129644403566793</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1628,7 +2806,7 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>1.3192534305471071</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +2817,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>43.740472843204657</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1650,7 +2828,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>11.920998173158736</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1659,12 +2837,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D9B140-C03F-4F25-A106-70754D386262}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,7 +2878,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1714,7 +2892,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1728,7 +2906,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1742,7 +2920,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1756,7 +2934,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1770,7 +2948,7 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1784,7 +2962,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1798,7 +2976,7 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1812,7 +2990,7 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1826,7 +3004,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1840,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1854,7 +3032,7 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1868,7 +3046,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,7 +3060,7 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,7 +3074,7 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1910,7 +3088,7 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,7 +3102,7 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1938,7 +3116,7 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,7 +3130,7 @@
         <v>10</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,7 +3144,7 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1980,7 +3158,7 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,7 +3172,7 @@
         <v>10</v>
       </c>
       <c r="D23">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2008,7 +3186,7 @@
         <v>10</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2022,7 +3200,7 @@
         <v>10</v>
       </c>
       <c r="D25">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2036,7 +3214,7 @@
         <v>10</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,7 +3228,7 @@
         <v>10</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2064,7 +3242,7 @@
         <v>10</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2078,7 +3256,7 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,7 +3270,7 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,7 +3284,7 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2120,7 +3298,7 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2134,7 +3312,7 @@
         <v>10</v>
       </c>
       <c r="D33">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2148,7 +3326,7 @@
         <v>10</v>
       </c>
       <c r="D34">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2162,7 +3340,7 @@
         <v>10</v>
       </c>
       <c r="D35">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2176,7 +3354,7 @@
         <v>10</v>
       </c>
       <c r="D36">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2190,7 +3368,7 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2204,7 +3382,7 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2218,7 +3396,7 @@
         <v>10</v>
       </c>
       <c r="D39">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2232,7 +3410,7 @@
         <v>10</v>
       </c>
       <c r="D40">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2246,7 +3424,7 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,7 +3438,7 @@
         <v>10</v>
       </c>
       <c r="D42">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2274,7 +3452,7 @@
         <v>10</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2288,7 +3466,7 @@
         <v>10</v>
       </c>
       <c r="D44">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2302,7 +3480,7 @@
         <v>10</v>
       </c>
       <c r="D45">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2316,7 +3494,7 @@
         <v>10</v>
       </c>
       <c r="D46">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2330,7 +3508,7 @@
         <v>10</v>
       </c>
       <c r="D47">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2344,7 +3522,7 @@
         <v>10</v>
       </c>
       <c r="D48">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2358,7 +3536,7 @@
         <v>10</v>
       </c>
       <c r="D49">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -2367,7 +3545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6732AF99-71C5-4774-AA47-E72551FC484C}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2406,12 +3584,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA7E102-6131-489B-B76D-85F559D2C626}">
   <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2779,7 +3957,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28FED19F-B52E-4B99-9DD7-59D5926AE3D0}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2822,7 +4000,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A161CE-62A0-4BFF-9974-63390BAAA1A2}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -2862,613 +4040,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD32A2A-87A0-4F8D-AE5A-93ADC2EEC530}">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>202201</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>202202</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>202203</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>202204</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>202205</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>202206</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>202207</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>202208</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>202209</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>202210</v>
-      </c>
-      <c r="B11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>202211</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>202212</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACFE55F3-700B-4740-9D96-DDF923385329}">
-  <dimension ref="A1:E25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>202201</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>202202</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>202203</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>202204</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>202205</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>202206</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>202207</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>202208</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>202209</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>202210</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>202211</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>202212</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>202201</v>
-      </c>
-      <c r="B14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>202202</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>202203</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>202204</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>202205</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>202206</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>202207</v>
-      </c>
-      <c r="B20" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>202208</v>
-      </c>
-      <c r="B21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>202209</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>202210</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>202211</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>202212</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25">
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed duration contracts implemented
</commit_message>
<xml_diff>
--- a/deterministic_2cust_2mills.xlsx
+++ b/deterministic_2cust_2mills.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Thesis\dev\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52A6F53-0BFF-43B2-B35E-96208C5D7E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E2D196-6464-467A-8E38-BB6EABC30361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14670" yWindow="1965" windowWidth="21600" windowHeight="14070" firstSheet="2" activeTab="2" xr2:uid="{B617CF86-C715-45AA-82CA-B7528EBD08D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="3" activeTab="11" xr2:uid="{B617CF86-C715-45AA-82CA-B7528EBD08D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Contracts" sheetId="14" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="31">
   <si>
     <t>CALMONTH</t>
   </si>
@@ -149,12 +149,6 @@
   </si>
   <si>
     <t>l3</t>
-  </si>
-  <si>
-    <t>forced fd</t>
-  </si>
-  <si>
-    <t>free</t>
   </si>
 </sst>
 </file>
@@ -641,10 +635,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCD32A2A-87A0-4F8D-AE5A-93ADC2EEC530}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +647,7 @@
     <col min="2" max="2" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -664,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>202201</v>
       </c>
@@ -672,10 +666,10 @@
         <v>10</v>
       </c>
       <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>202202</v>
       </c>
@@ -686,7 +680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>202203</v>
       </c>
@@ -697,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>202204</v>
       </c>
@@ -708,7 +702,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>202205</v>
       </c>
@@ -719,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>202206</v>
       </c>
@@ -730,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>202207</v>
       </c>
@@ -741,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>202208</v>
       </c>
@@ -752,7 +746,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>202209</v>
       </c>
@@ -763,7 +757,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>202210</v>
       </c>
@@ -774,7 +768,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>202211</v>
       </c>
@@ -785,7 +779,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>202212</v>
       </c>
@@ -794,28 +788,6 @@
       </c>
       <c r="C13">
         <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E15" t="s">
-        <v>31</v>
-      </c>
-      <c r="F15">
-        <v>-37969.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16">
-        <v>-37669.5</v>
-      </c>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18">
-        <f>F15-F16</f>
-        <v>-300</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +1649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7E0AE82-9F3D-4041-B085-9F4202728AA7}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -2718,8 +2690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967FF54E-DED1-4824-B739-3FC722291D17}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2752,7 +2724,7 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2766,7 +2738,7 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2780,7 +2752,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2794,7 +2766,7 @@
         <v>10</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2808,7 +2780,7 @@
         <v>10</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2822,7 +2794,7 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2836,7 +2808,7 @@
         <v>10</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2850,7 +2822,7 @@
         <v>10</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2864,7 +2836,7 @@
         <v>10</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2878,7 +2850,7 @@
         <v>10</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2892,7 +2864,7 @@
         <v>10</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2906,7 +2878,7 @@
         <v>10</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2920,7 +2892,7 @@
         <v>10</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2934,7 +2906,7 @@
         <v>10</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2948,7 +2920,7 @@
         <v>10</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2962,7 +2934,7 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2976,7 +2948,7 @@
         <v>10</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2990,7 +2962,7 @@
         <v>10</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3004,7 +2976,7 @@
         <v>10</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3018,7 +2990,7 @@
         <v>10</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3032,7 +3004,7 @@
         <v>10</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3046,7 +3018,7 @@
         <v>10</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -3060,7 +3032,7 @@
         <v>10</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3074,7 +3046,7 @@
         <v>10</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3088,7 +3060,7 @@
         <v>10</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3102,7 +3074,7 @@
         <v>10</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3116,7 +3088,7 @@
         <v>10</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3130,7 +3102,7 @@
         <v>10</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3144,7 +3116,7 @@
         <v>10</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -3158,7 +3130,7 @@
         <v>10</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -3172,7 +3144,7 @@
         <v>10</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -3186,7 +3158,7 @@
         <v>10</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -3200,7 +3172,7 @@
         <v>10</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -3214,7 +3186,7 @@
         <v>10</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3228,7 +3200,7 @@
         <v>10</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -3242,7 +3214,7 @@
         <v>10</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -3256,7 +3228,7 @@
         <v>10</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -3270,7 +3242,7 @@
         <v>10</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -3284,7 +3256,7 @@
         <v>10</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -3298,7 +3270,7 @@
         <v>10</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3312,7 +3284,7 @@
         <v>10</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,7 +3298,7 @@
         <v>10</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3340,7 +3312,7 @@
         <v>10</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -3354,7 +3326,7 @@
         <v>10</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3368,7 +3340,7 @@
         <v>10</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -3382,7 +3354,7 @@
         <v>10</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -3396,7 +3368,7 @@
         <v>10</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -3410,7 +3382,7 @@
         <v>10</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3424,7 +3396,7 @@
         <v>10</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3438,7 +3410,7 @@
         <v>10</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3452,7 +3424,7 @@
         <v>10</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3466,7 +3438,7 @@
         <v>10</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -3480,7 +3452,7 @@
         <v>10</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3494,7 +3466,7 @@
         <v>10</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -3508,7 +3480,7 @@
         <v>10</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3522,7 +3494,7 @@
         <v>10</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3536,7 +3508,7 @@
         <v>10</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3550,7 +3522,7 @@
         <v>10</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -3564,7 +3536,7 @@
         <v>10</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -3578,7 +3550,7 @@
         <v>10</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3592,7 +3564,7 @@
         <v>10</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3606,7 +3578,7 @@
         <v>10</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3620,7 +3592,7 @@
         <v>10</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -3634,7 +3606,7 @@
         <v>10</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -3648,7 +3620,7 @@
         <v>10</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3662,7 +3634,7 @@
         <v>10</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3676,7 +3648,7 @@
         <v>10</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3690,7 +3662,7 @@
         <v>10</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3704,7 +3676,7 @@
         <v>10</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -3718,7 +3690,7 @@
         <v>10</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3732,7 +3704,7 @@
         <v>10</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -3746,7 +3718,7 @@
         <v>10</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>